<commit_message>
coloring fields and field width and other style
</commit_message>
<xml_diff>
--- a/combined_metadata_template.xlsx
+++ b/combined_metadata_template.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata Template Sequencing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="MetaDataTemplate" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Database" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,13 +26,34 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
+        <bgColor rgb="00FFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -47,8 +68,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,888 +447,958 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Select an Option</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Key</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Example_Value</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Example Value</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Controlled Vocabulary / Value Restrictions</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Resource Link(s)</t>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Controlled_Vocabulary/Value-Restrictions</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Resource_Link(s)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Study Information</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr"/>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Analysis of Intestinal Crypt, Villus, and Polyp Cells</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>A concise title describing the overall study</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Analysis of Intestinal Crypt, Villus, and Polyp Cells</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>Free text; consider limiting length (e.g., ≤250 characters)</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Study Information</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Summary / Abstract</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Summary/Abstract</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr"/>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>This study investigates transcriptomic changes under infection conditions.</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Detailed study summary and objectives</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>This study investigates transcriptomic changes under infection conditions.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>Free text; follow standard writing guidelines</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Study Information</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Experimental Design</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Experimental_Design</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr"/>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>RNA-seq of single cells comparing infected vs. control conditions.</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>Overview of study design including factors, controls, and replicates</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>RNA-seq of single cells comparing infected vs. control conditions.</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>Free text; consider using standardized descriptors if available</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
         <is>
           <t>https://www.ebi.ac.uk/arrayexpress/help/</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Sample Identifier</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Sample_Identifier</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr"/>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>RNA-Seq_Sample_001</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>Unique identifier for each biological sample</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>RNA-Seq_Sample_001</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>Must be unique; use an alphanumeric/underscore format (e.g., regex: ^[A-Za-z0-9_]+$)</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>Organism</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr"/>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>Pseudomonas aeruginosa</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>Species name from which the sample is derived</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Pseudomonas aeruginosa</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
         <is>
           <t>Must conform to NCBI Taxonomy names</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" s="3" t="inlineStr">
         <is>
           <t>https://www.ncbi.nlm.nih.gov/Taxonomy/taxonomyhome.html</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Tissue / Cell Type</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Specific tissue, cell line, or cell type of origin</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Tissue</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr"/>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>Pancreas</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>Specific tissue</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>Use controlled terms from ontologies such as Uberon or Cell Ontology</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>http://www.ontobee.org/</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>Sample Information</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Cell_Type</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr"/>
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>HeLa cells</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>Specific cell line, or cell type of origin</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
         <is>
           <t>Use controlled terms from ontologies such as Uberon or Cell Ontology</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G8" s="3" t="inlineStr">
         <is>
           <t>http://www.ontobee.org/</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Strain Identifier</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Strain_Identifier</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr"/>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>JCM 14847</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="inlineStr">
         <is>
           <t>Strain information (if applicable)</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>JCM 14847</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+      <c r="F9" s="3" t="inlineStr">
         <is>
           <t>Use recognized strain IDs (e.g., from ATCC, DSMZ)</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G9" s="3" t="inlineStr">
         <is>
           <t>https://www.atcc.org/</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Collection Date</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Collection_Date</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr"/>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>2025-03-24</t>
+        </is>
+      </c>
+      <c r="E10" s="3" t="inlineStr">
         <is>
           <t>Date on which the sample was collected</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>2025-03-24</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="F10" s="3" t="inlineStr">
         <is>
           <t>Must follow ISO 8601 format (YYYY-MM-DD)</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G10" s="3" t="inlineStr">
         <is>
           <t>https://www.iso.org/iso-8601-date-and-time-format.html</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Experimental Conditions</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Treatment Conditions</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>Treatment_Conditions</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr"/>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Anti-Grem1 antibody treatment</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>Description of the experimental treatment(s) or conditions applied</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Anti-Grem1 antibody treatment</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="F11" s="2" t="inlineStr">
         <is>
           <t>If available, select from a controlled list (e.g., EFO terms)</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G11" s="2" t="inlineStr">
         <is>
           <t>https://www.ebi.ac.uk/efo/</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>Experimental Conditions</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Treatment Duration</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Treatment_Duration</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr"/>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>10 weeks</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>Duration for which the treatment was applied</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>10 weeks</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
+      <c r="F12" s="2" t="inlineStr">
         <is>
           <t>Numeric value with a unit; standardize unit selection (e.g., hours, days, weeks)</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G12" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Experimental Conditions</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>Concentration</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" s="2" t="inlineStr"/>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>30 mg/kg</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
         <is>
           <t>Concentration or dosage of the treatment agent</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>30 mg/kg</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
+      <c r="F13" s="2" t="inlineStr">
         <is>
           <t>Numeric value with unit; ensure consistency across samples</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G13" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Library Preparation Method</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Library_Preparation_Method</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr"/>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>TruSeq Stranded mRNA Library Prep Kit</t>
+        </is>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
         <is>
           <t>Method or kit used for nucleic acid library preparation</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>TruSeq Stranded mRNA Library Prep Kit</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="F14" s="3" t="inlineStr">
         <is>
           <t>Use a predefined list from vendor documentation or internal standards</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G14" s="3" t="inlineStr">
         <is>
           <t>https://www.illumina.com/</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Sequencing Platform</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Sequencing_Platform</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr"/>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>Illumina NovaSeq</t>
+        </is>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
         <is>
           <t>Instrument or platform used for sequencing</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Illumina NovaSeq</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
+      <c r="F15" s="3" t="inlineStr">
         <is>
           <t>Must be selected from a controlled list (e.g., Illumina, PacBio, Oxford Nanopore)</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G15" s="3" t="inlineStr">
         <is>
           <t>https://www.ncbi.nlm.nih.gov/sra/docs/submitdesign/</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Sequencing Depth</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Sequencing_Depth</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr"/>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>50 million reads</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
         <is>
           <t>Number of reads obtained or overall depth of sequencing</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>50 million reads</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="F16" s="3" t="inlineStr">
         <is>
           <t>Free numeric text; standard units should be used</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G16" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Single or Paired-End</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Single_or_Paired-End</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr"/>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>Paired-end</t>
+        </is>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
         <is>
           <t>Specifies whether the sequencing was single-end or paired-end</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Paired-end</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
+      <c r="F17" s="3" t="inlineStr">
         <is>
           <t>Allowed values: Single-end, Paired-end</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G17" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Instrument Model</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Instrument_Model</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr"/>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>Illumina HiSeq 2000</t>
+        </is>
+      </c>
+      <c r="E18" s="3" t="inlineStr">
         <is>
           <t>Specific model of the sequencing instrument</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Illumina HiSeq 2000</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="F18" s="3" t="inlineStr">
         <is>
           <t>Use a controlled list (as provided by the manufacturer)</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G18" s="3" t="inlineStr">
         <is>
           <t>https://www.illumina.com/systems/sequencing-platforms.html</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Quality Control Metrics</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Quality_Control_Metrics</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr"/>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>RIN &gt; 8, Q30 &gt; 85%</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
         <is>
           <t>Key quality metrics such as RNA integrity number and quality scores</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>RIN &gt; 8, Q30 &gt; 85%</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
+      <c r="F19" s="3" t="inlineStr">
         <is>
           <t>Free numeric values; standardize units and thresholds</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G19" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>Bioinformatics Analysis</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Read Alignment Algorithm</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Read_Alignment_Algorithm</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr"/>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>HISAT2</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
         <is>
           <t>Software used for aligning reads to the reference genome</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>HISAT2</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
+      <c r="F20" s="2" t="inlineStr">
         <is>
           <t>Choose from a controlled list (e.g., HISAT2, STAR, Bowtie2)</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G20" s="2" t="inlineStr">
         <is>
           <t>https://github.com/ewels/MultiQC</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>Bioinformatics Analysis</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Genome Reference</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>Genome_Reference</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr"/>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>Pseudomonas aeruginosa PAO1</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
         <is>
           <t>Reference genome or assembly used for analysis</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Pseudomonas aeruginosa PAO1</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
+      <c r="F21" s="2" t="inlineStr">
         <is>
           <t>Must match identifiers from recognized genome databases</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G21" s="2" t="inlineStr">
         <is>
           <t>https://www.ncbi.nlm.nih.gov/assembly/</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Bioinformatics Analysis</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Differential Expression Analysis</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>Differential_Expression_Analysis</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr"/>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>DESeq2 with FDR &lt; 0.05</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
         <is>
           <t>Software and statistical thresholds used for differential expression analysis</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>DESeq2 with FDR &lt; 0.05</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
+      <c r="F22" s="2" t="inlineStr">
         <is>
           <t>Choose from accepted tools (e.g., DESeq2, edgeR, limma)</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G22" s="2" t="inlineStr">
         <is>
           <t>https://bioconductor.org/packages/release/bioc/html/DESeq2.html</t>
         </is>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Bioinformatics Analysis</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Gene Annotation</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>Gene_Annotation</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr"/>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>Ensembl, KEGG</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>Databases or methods used for gene functional annotation</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Ensembl, KEGG</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
+      <c r="F23" s="2" t="inlineStr">
         <is>
           <t>Use controlled database names; if possible, select from a predefined list</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G23" s="2" t="inlineStr">
         <is>
           <t>https://www.ensembl.org/</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="24">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>Ethical &amp; Legal</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Ethical Approval</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Ethical_Approval</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr"/>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>IRB #12345</t>
+        </is>
+      </c>
+      <c r="E24" s="3" t="inlineStr">
         <is>
           <t>Details regarding ethics committee or IRB approval</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>IRB #12345</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
+      <c r="F24" s="3" t="inlineStr">
         <is>
           <t>Free text; may follow a predefined institutional format</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G24" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>Ethical &amp; Legal</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Data Sharing Policy</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>Data_Sharing_Policy</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr"/>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>Data available under CC-BY 4.0</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
         <is>
           <t>Conditions or restrictions related to data sharing</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Data available under CC-BY 4.0</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
+      <c r="F25" s="3" t="inlineStr">
         <is>
           <t>Must be selected from a controlled list of licensing options</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G25" s="3" t="inlineStr">
         <is>
           <t>https://creativecommons.org/licenses/by/4.0/</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>Contact Information</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Contributor / Contact Name</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>Contributor/Contact_Name</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr"/>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
         <is>
           <t>Primary contact or contributor for the study</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Jane Doe</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
+      <c r="F26" s="2" t="inlineStr">
         <is>
           <t>Free text; consider enforcing a 'Last Name, First Name' format</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G26" s="2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Contact Information</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Contact Email</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>Contact_Email</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr"/>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>jane.doe@example.com</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
         <is>
           <t>Email address of the study contact</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>jane.doe@example.com</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
+      <c r="F27" s="2" t="inlineStr">
         <is>
           <t>Must follow standard email format</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G27" s="2" t="inlineStr">
         <is>
           <t>https://html.spec.whatwg.org/multipage/input.html#valid-e-mail-address</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>Contact Information</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Contact Affiliation</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>Contact_Affiliation</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr"/>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>Example University</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
         <is>
           <t>Affiliation or institution of the study contact</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Example University</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
+      <c r="F28" s="2" t="inlineStr">
         <is>
           <t>Free text; optionally choose from a controlled list if available</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G28" s="2" t="inlineStr">
         <is>
           <t>https://grid.ac/</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation sqref="D6" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=Database!$E$2:$E$4</formula1>
     </dataValidation>
-    <dataValidation sqref="D16" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="D17" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=Database!$O$2:$O$3</formula1>
-    </dataValidation>
-    <dataValidation sqref="A1" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Option1,Option2,Option3"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1315,165 +1418,193 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="25" customWidth="1" min="11" max="11"/>
+    <col width="25" customWidth="1" min="12" max="12"/>
+    <col width="25" customWidth="1" min="13" max="13"/>
+    <col width="25" customWidth="1" min="14" max="14"/>
+    <col width="25" customWidth="1" min="15" max="15"/>
+    <col width="25" customWidth="1" min="16" max="16"/>
+    <col width="25" customWidth="1" min="17" max="17"/>
+    <col width="25" customWidth="1" min="18" max="18"/>
+    <col width="25" customWidth="1" min="19" max="19"/>
+    <col width="25" customWidth="1" min="20" max="20"/>
+    <col width="25" customWidth="1" min="21" max="21"/>
+    <col width="25" customWidth="1" min="22" max="22"/>
+    <col width="25" customWidth="1" min="23" max="23"/>
+    <col width="25" customWidth="1" min="24" max="24"/>
+    <col width="25" customWidth="1" min="25" max="25"/>
+    <col width="25" customWidth="1" min="26" max="26"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Summary / Abstract</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Experimental Design</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Sample Identifier</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Organism</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Tissue / Cell Type</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Strain Identifier</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Collection Date</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Treatment Conditions</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Treatment Duration</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Concentration</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Library Preparation Method</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Sequencing Platform</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Sequencing Depth</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Single or Paired-End</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Instrument Model</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Quality Control Metrics</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Read Alignment Algorithm</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Genome Reference</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Differential Expression Analysis</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Gene Annotation</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Ethical Approval</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Data Sharing Policy</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Contributor / Contact Name</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Contact Email</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Contact Affiliation</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O2" s="4" t="inlineStr">
         <is>
           <t>Single-end</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="4" t="inlineStr">
         <is>
           <t>Pseudomonas aeruginosa</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O3" s="4" t="inlineStr">
         <is>
           <t>Paired-end</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
         <is>
           <t>Mus musculus</t>
         </is>

</xml_diff>

<commit_message>
established drop down menu. Now dowload an parse database
</commit_message>
<xml_diff>
--- a/combined_metadata_template.xlsx
+++ b/combined_metadata_template.xlsx
@@ -10,7 +10,10 @@
     <sheet name="MetaDataTemplate" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Database" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="OrganismList">Database!$E$2:$E$4</definedName>
+    <definedName name="SPEList">Database!$O$2:$O$3</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -76,10 +79,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -453,7 +456,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
@@ -507,28 +510,28 @@
           <t>Study Information</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr"/>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr"/>
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>Analysis of Intestinal Crypt, Villus, and Polyp Cells</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>A concise title describing the overall study</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>Free text; consider limiting length (e.g., ≤250 characters)</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -540,28 +543,28 @@
           <t>Study Information</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Summary/Abstract</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr"/>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr"/>
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>This study investigates transcriptomic changes under infection conditions.</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>Detailed study summary and objectives</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>Free text; follow standard writing guidelines</t>
         </is>
       </c>
-      <c r="G3" s="2" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -573,35 +576,35 @@
           <t>Study Information</t>
         </is>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Experimental_Design</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr"/>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr"/>
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>RNA-seq of single cells comparing infected vs. control conditions.</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>Overview of study design including factors, controls, and replicates</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>Free text; consider using standardized descriptors if available</t>
         </is>
       </c>
-      <c r="G4" s="2" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>https://www.ebi.ac.uk/arrayexpress/help/</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
@@ -634,7 +637,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
@@ -667,7 +670,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
@@ -700,7 +703,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
@@ -733,7 +736,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="4" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
@@ -766,7 +769,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Sample Information</t>
         </is>
@@ -804,28 +807,28 @@
           <t>Experimental Conditions</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>Treatment_Conditions</t>
         </is>
       </c>
-      <c r="C11" s="2" t="inlineStr"/>
-      <c r="D11" s="2" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr"/>
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>Anti-Grem1 antibody treatment</t>
         </is>
       </c>
-      <c r="E11" s="2" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Description of the experimental treatment(s) or conditions applied</t>
         </is>
       </c>
-      <c r="F11" s="2" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
         <is>
           <t>If available, select from a controlled list (e.g., EFO terms)</t>
         </is>
       </c>
-      <c r="G11" s="2" t="inlineStr">
+      <c r="G11" s="3" t="inlineStr">
         <is>
           <t>https://www.ebi.ac.uk/efo/</t>
         </is>
@@ -837,28 +840,28 @@
           <t>Experimental Conditions</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>Treatment_Duration</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr"/>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr"/>
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>10 weeks</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
+      <c r="E12" s="3" t="inlineStr">
         <is>
           <t>Duration for which the treatment was applied</t>
         </is>
       </c>
-      <c r="F12" s="2" t="inlineStr">
+      <c r="F12" s="3" t="inlineStr">
         <is>
           <t>Numeric value with a unit; standardize unit selection (e.g., hours, days, weeks)</t>
         </is>
       </c>
-      <c r="G12" s="2" t="inlineStr">
+      <c r="G12" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -870,35 +873,35 @@
           <t>Experimental Conditions</t>
         </is>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
         <is>
           <t>Concentration</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr"/>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr"/>
+      <c r="D13" s="3" t="inlineStr">
         <is>
           <t>30 mg/kg</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
+      <c r="E13" s="3" t="inlineStr">
         <is>
           <t>Concentration or dosage of the treatment agent</t>
         </is>
       </c>
-      <c r="F13" s="2" t="inlineStr">
+      <c r="F13" s="3" t="inlineStr">
         <is>
           <t>Numeric value with unit; ensure consistency across samples</t>
         </is>
       </c>
-      <c r="G13" s="2" t="inlineStr">
+      <c r="G13" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="4" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
@@ -931,7 +934,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" s="4" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
@@ -964,7 +967,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="inlineStr">
+      <c r="A16" s="4" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
@@ -997,7 +1000,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="inlineStr">
+      <c r="A17" s="4" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
@@ -1030,7 +1033,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="inlineStr">
+      <c r="A18" s="4" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
@@ -1063,7 +1066,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="inlineStr">
+      <c r="A19" s="4" t="inlineStr">
         <is>
           <t>Sequencing Details</t>
         </is>
@@ -1101,28 +1104,28 @@
           <t>Bioinformatics Analysis</t>
         </is>
       </c>
-      <c r="B20" s="2" t="inlineStr">
+      <c r="B20" s="3" t="inlineStr">
         <is>
           <t>Read_Alignment_Algorithm</t>
         </is>
       </c>
-      <c r="C20" s="2" t="inlineStr"/>
-      <c r="D20" s="2" t="inlineStr">
+      <c r="C20" s="3" t="inlineStr"/>
+      <c r="D20" s="3" t="inlineStr">
         <is>
           <t>HISAT2</t>
         </is>
       </c>
-      <c r="E20" s="2" t="inlineStr">
+      <c r="E20" s="3" t="inlineStr">
         <is>
           <t>Software used for aligning reads to the reference genome</t>
         </is>
       </c>
-      <c r="F20" s="2" t="inlineStr">
+      <c r="F20" s="3" t="inlineStr">
         <is>
           <t>Choose from a controlled list (e.g., HISAT2, STAR, Bowtie2)</t>
         </is>
       </c>
-      <c r="G20" s="2" t="inlineStr">
+      <c r="G20" s="3" t="inlineStr">
         <is>
           <t>https://github.com/ewels/MultiQC</t>
         </is>
@@ -1134,28 +1137,28 @@
           <t>Bioinformatics Analysis</t>
         </is>
       </c>
-      <c r="B21" s="2" t="inlineStr">
+      <c r="B21" s="3" t="inlineStr">
         <is>
           <t>Genome_Reference</t>
         </is>
       </c>
-      <c r="C21" s="2" t="inlineStr"/>
-      <c r="D21" s="2" t="inlineStr">
+      <c r="C21" s="3" t="inlineStr"/>
+      <c r="D21" s="3" t="inlineStr">
         <is>
           <t>Pseudomonas aeruginosa PAO1</t>
         </is>
       </c>
-      <c r="E21" s="2" t="inlineStr">
+      <c r="E21" s="3" t="inlineStr">
         <is>
           <t>Reference genome or assembly used for analysis</t>
         </is>
       </c>
-      <c r="F21" s="2" t="inlineStr">
+      <c r="F21" s="3" t="inlineStr">
         <is>
           <t>Must match identifiers from recognized genome databases</t>
         </is>
       </c>
-      <c r="G21" s="2" t="inlineStr">
+      <c r="G21" s="3" t="inlineStr">
         <is>
           <t>https://www.ncbi.nlm.nih.gov/assembly/</t>
         </is>
@@ -1167,28 +1170,28 @@
           <t>Bioinformatics Analysis</t>
         </is>
       </c>
-      <c r="B22" s="2" t="inlineStr">
+      <c r="B22" s="3" t="inlineStr">
         <is>
           <t>Differential_Expression_Analysis</t>
         </is>
       </c>
-      <c r="C22" s="2" t="inlineStr"/>
-      <c r="D22" s="2" t="inlineStr">
+      <c r="C22" s="3" t="inlineStr"/>
+      <c r="D22" s="3" t="inlineStr">
         <is>
           <t>DESeq2 with FDR &lt; 0.05</t>
         </is>
       </c>
-      <c r="E22" s="2" t="inlineStr">
+      <c r="E22" s="3" t="inlineStr">
         <is>
           <t>Software and statistical thresholds used for differential expression analysis</t>
         </is>
       </c>
-      <c r="F22" s="2" t="inlineStr">
+      <c r="F22" s="3" t="inlineStr">
         <is>
           <t>Choose from accepted tools (e.g., DESeq2, edgeR, limma)</t>
         </is>
       </c>
-      <c r="G22" s="2" t="inlineStr">
+      <c r="G22" s="3" t="inlineStr">
         <is>
           <t>https://bioconductor.org/packages/release/bioc/html/DESeq2.html</t>
         </is>
@@ -1200,35 +1203,35 @@
           <t>Bioinformatics Analysis</t>
         </is>
       </c>
-      <c r="B23" s="2" t="inlineStr">
+      <c r="B23" s="3" t="inlineStr">
         <is>
           <t>Gene_Annotation</t>
         </is>
       </c>
-      <c r="C23" s="2" t="inlineStr"/>
-      <c r="D23" s="2" t="inlineStr">
+      <c r="C23" s="3" t="inlineStr"/>
+      <c r="D23" s="3" t="inlineStr">
         <is>
           <t>Ensembl, KEGG</t>
         </is>
       </c>
-      <c r="E23" s="2" t="inlineStr">
+      <c r="E23" s="3" t="inlineStr">
         <is>
           <t>Databases or methods used for gene functional annotation</t>
         </is>
       </c>
-      <c r="F23" s="2" t="inlineStr">
+      <c r="F23" s="3" t="inlineStr">
         <is>
           <t>Use controlled database names; if possible, select from a predefined list</t>
         </is>
       </c>
-      <c r="G23" s="2" t="inlineStr">
+      <c r="G23" s="3" t="inlineStr">
         <is>
           <t>https://www.ensembl.org/</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+      <c r="A24" s="4" t="inlineStr">
         <is>
           <t>Ethical &amp; Legal</t>
         </is>
@@ -1261,7 +1264,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="inlineStr">
+      <c r="A25" s="4" t="inlineStr">
         <is>
           <t>Ethical &amp; Legal</t>
         </is>
@@ -1299,28 +1302,28 @@
           <t>Contact Information</t>
         </is>
       </c>
-      <c r="B26" s="2" t="inlineStr">
+      <c r="B26" s="3" t="inlineStr">
         <is>
           <t>Contributor/Contact_Name</t>
         </is>
       </c>
-      <c r="C26" s="2" t="inlineStr"/>
-      <c r="D26" s="2" t="inlineStr">
+      <c r="C26" s="3" t="inlineStr"/>
+      <c r="D26" s="3" t="inlineStr">
         <is>
           <t>Jane Doe</t>
         </is>
       </c>
-      <c r="E26" s="2" t="inlineStr">
+      <c r="E26" s="3" t="inlineStr">
         <is>
           <t>Primary contact or contributor for the study</t>
         </is>
       </c>
-      <c r="F26" s="2" t="inlineStr">
+      <c r="F26" s="3" t="inlineStr">
         <is>
           <t>Free text; consider enforcing a 'Last Name, First Name' format</t>
         </is>
       </c>
-      <c r="G26" s="2" t="inlineStr">
+      <c r="G26" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1332,28 +1335,28 @@
           <t>Contact Information</t>
         </is>
       </c>
-      <c r="B27" s="2" t="inlineStr">
+      <c r="B27" s="3" t="inlineStr">
         <is>
           <t>Contact_Email</t>
         </is>
       </c>
-      <c r="C27" s="2" t="inlineStr"/>
-      <c r="D27" s="2" t="inlineStr">
+      <c r="C27" s="3" t="inlineStr"/>
+      <c r="D27" s="3" t="inlineStr">
         <is>
           <t>jane.doe@example.com</t>
         </is>
       </c>
-      <c r="E27" s="2" t="inlineStr">
+      <c r="E27" s="3" t="inlineStr">
         <is>
           <t>Email address of the study contact</t>
         </is>
       </c>
-      <c r="F27" s="2" t="inlineStr">
+      <c r="F27" s="3" t="inlineStr">
         <is>
           <t>Must follow standard email format</t>
         </is>
       </c>
-      <c r="G27" s="2" t="inlineStr">
+      <c r="G27" s="3" t="inlineStr">
         <is>
           <t>https://html.spec.whatwg.org/multipage/input.html#valid-e-mail-address</t>
         </is>
@@ -1365,40 +1368,52 @@
           <t>Contact Information</t>
         </is>
       </c>
-      <c r="B28" s="2" t="inlineStr">
+      <c r="B28" s="3" t="inlineStr">
         <is>
           <t>Contact_Affiliation</t>
         </is>
       </c>
-      <c r="C28" s="2" t="inlineStr"/>
-      <c r="D28" s="2" t="inlineStr">
+      <c r="C28" s="3" t="inlineStr"/>
+      <c r="D28" s="3" t="inlineStr">
         <is>
           <t>Example University</t>
         </is>
       </c>
-      <c r="E28" s="2" t="inlineStr">
+      <c r="E28" s="3" t="inlineStr">
         <is>
           <t>Affiliation or institution of the study contact</t>
         </is>
       </c>
-      <c r="F28" s="2" t="inlineStr">
+      <c r="F28" s="3" t="inlineStr">
         <is>
           <t>Free text; optionally choose from a controlled list if available</t>
         </is>
       </c>
-      <c r="G28" s="2" t="inlineStr">
+      <c r="G28" s="3" t="inlineStr">
         <is>
           <t>https://grid.ac/</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="D6" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Database!$E$2:$E$4</formula1>
+  <dataValidations count="6">
+    <dataValidation sqref="C6" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=OrganismList</formula1>
     </dataValidation>
-    <dataValidation sqref="D17" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>=Database!$O$2:$O$3</formula1>
+    <dataValidation sqref="C17" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=SPEList</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=OrganismList</formula1>
+    </dataValidation>
+    <dataValidation sqref="C17" showDropDown="1" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=SPEList</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=OrganismList</formula1>
+    </dataValidation>
+    <dataValidation sqref="C17" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=SPEList</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1417,7 +1432,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="25" customWidth="1" min="2" max="2"/>
@@ -1455,7 +1470,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Summary / Abstract</t>
+          <t>Summary/Abstract</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -1475,7 +1490,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Tissue / Cell Type</t>
+          <t>Tissue/Cell Type</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -1565,7 +1580,7 @@
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Contributor / Contact Name</t>
+          <t>Contributor/Contact Name</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
@@ -1580,31 +1595,31 @@
       </c>
     </row>
     <row r="2">
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>Homo sapiens</t>
         </is>
       </c>
-      <c r="O2" s="4" t="inlineStr">
+      <c r="O2" s="3" t="inlineStr">
         <is>
           <t>Single-end</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>Pseudomonas aeruginosa</t>
         </is>
       </c>
-      <c r="O3" s="4" t="inlineStr">
+      <c r="O3" s="3" t="inlineStr">
         <is>
           <t>Paired-end</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>Mus musculus</t>
         </is>

</xml_diff>